<commit_message>
Exam 2 Review Started
</commit_message>
<xml_diff>
--- a/SE-4367.0U1-Testing/Grades/Grades.xlsx
+++ b/SE-4367.0U1-Testing/Grades/Grades.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1830" windowWidth="28755" windowHeight="12840"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="28755" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D14" sqref="D12:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,11 +702,11 @@
       </c>
       <c r="C6" s="8">
         <f t="shared" ref="C6:H6" si="0">COUNT(C8:C21)</f>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6" s="8">
         <f t="shared" si="0"/>
@@ -714,7 +714,7 @@
       </c>
       <c r="F6" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G6" s="8">
         <f t="shared" si="0"/>
@@ -737,11 +737,11 @@
       </c>
       <c r="C7" s="22">
         <f t="shared" ref="C7:H7" si="1">IF(C6&lt;&gt;0,IF(C5&lt;&gt;0,(SUM(C8:C21)/C6)*C5,0), 0)</f>
-        <v>0.12857142857142856</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
-        <v>0.19228571428571431</v>
+        <v>0.1865</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
@@ -749,7 +749,7 @@
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>0.24400000000000002</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="1"/>
@@ -762,7 +762,7 @@
       <c r="I7" s="5"/>
       <c r="J7">
         <f>SUM(C7:H7)</f>
-        <v>0.87985714285714289</v>
+        <v>0.83416666666666672</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -860,13 +860,9 @@
       <c r="C12" s="21">
         <v>1</v>
       </c>
-      <c r="D12" s="11">
-        <v>1</v>
-      </c>
+      <c r="D12" s="11"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12">
-        <v>1</v>
-      </c>
+      <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="2"/>
@@ -881,13 +877,9 @@
       <c r="C13" s="21">
         <v>1</v>
       </c>
-      <c r="D13" s="11">
-        <v>1</v>
-      </c>
+      <c r="D13" s="11"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="12">
-        <v>1</v>
-      </c>
+      <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="2"/>
@@ -902,9 +894,7 @@
       <c r="C14" s="21">
         <v>1</v>
       </c>
-      <c r="D14" s="11">
-        <v>1</v>
-      </c>
+      <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -952,9 +942,7 @@
       <c r="B17" s="6">
         <v>10</v>
       </c>
-      <c r="C17" s="12">
-        <v>1</v>
-      </c>
+      <c r="C17" s="12"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -969,9 +957,7 @@
       <c r="B18" s="6">
         <v>11</v>
       </c>
-      <c r="C18" s="12">
-        <v>1</v>
-      </c>
+      <c r="C18" s="12"/>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -986,9 +972,7 @@
       <c r="B19" s="6">
         <v>12</v>
       </c>
-      <c r="C19" s="12">
-        <v>1</v>
-      </c>
+      <c r="C19" s="12"/>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -1003,9 +987,7 @@
       <c r="B20" s="6">
         <v>13</v>
       </c>
-      <c r="C20" s="12">
-        <v>1</v>
-      </c>
+      <c r="C20" s="12"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -1020,9 +1002,7 @@
       <c r="B21" s="4">
         <v>14</v>
       </c>
-      <c r="C21" s="14">
-        <v>1</v>
-      </c>
+      <c r="C21" s="14"/>
       <c r="D21" s="13"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>

</xml_diff>